<commit_message>
Final code worked as team
</commit_message>
<xml_diff>
--- a/Team01_WebScrapers_Dec2024/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/Team01_WebScrapers_Dec2024/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -5,20 +5,20 @@
   <sheets>
     <sheet state="visible" name="Final list for LFV Elimination " sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Final list for LCHFElimination " sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Filter -1 Allergies - Bonus Poi" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Final List for Allergies" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="7ajz6yix6MUPD6VUXpbLeAfnWoh6BpXwoCQ3QmgQ0Gw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="zieL8zQES7Yo3tj4vXBSFNCmrze3OhwGJpGaZZx3YfI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="250">
   <si>
     <t xml:space="preserve">Meal plan for Low Fat Vegan diet </t>
   </si>
@@ -746,7 +746,7 @@
     <t>pea</t>
   </si>
   <si>
-    <t>Allergies (Bonus points)</t>
+    <t>Allergies</t>
   </si>
   <si>
     <t>Milk</t>
@@ -913,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -932,6 +932,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -4868,76 +4871,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="12" t="s">
+    <row r="4">
+      <c r="A4" s="13" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="12" t="s">
+    <row r="5">
+      <c r="A5" s="13" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="12" t="s">
+    <row r="6">
+      <c r="A6" s="13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="12" t="s">
+    <row r="7">
+      <c r="A7" s="13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="12" t="s">
+    <row r="8">
+      <c r="A8" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="12" t="s">
+    <row r="9">
+      <c r="A9" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="12" t="s">
+    <row r="10">
+      <c r="A10" s="13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="12" t="s">
+    <row r="11">
+      <c r="A11" s="13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="12" t="s">
+    <row r="12">
+      <c r="A12" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="12" t="s">
+    <row r="13">
+      <c r="A13" s="13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="12" t="s">
+    <row r="14">
+      <c r="A14" s="13" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="12" t="s">
+    <row r="15">
+      <c r="A15" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -5917,6 +5924,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>